<commit_message>
Updated Items, Troops, and Skills.xlsx with various translations.
</commit_message>
<xml_diff>
--- a/data/Armors.xlsx
+++ b/data/Armors.xlsx
@@ -165,7 +165,7 @@
   </si>
   <si>
     <t>A dildo as quick as the wind
-Sex toys Physical strength consumption -10%</t>
+Sex toys HP consumption -10%</t>
   </si>
   <si>
     <t>&lt;mat1:A2*1&gt;
@@ -979,7 +979,7 @@
   </si>
   <si>
     <t>Legendary dildo
-Sex toys, physical strength consumption 0, 2 attacks</t>
+Sex toys, HP consumption 0, 2 attacks</t>
   </si>
   <si>
     <t xml:space="preserve">&lt;mat1:A53*1&gt;
@@ -1008,7 +1008,7 @@
   </si>
   <si>
     <t>Telescopic rod
-Sex toys Physical strength consumption -10%</t>
+Sex toys HP consumption -10%</t>
   </si>
   <si>
     <t>マンイーター</t>
@@ -1185,7 +1185,7 @@
   </si>
   <si>
     <t>Vibe that evaporates water with super vibration
-Sex toy water attribute special effect consumption physical strength -50%</t>
+Sex toy water attribute special effect consumption HP -50%</t>
   </si>
   <si>
     <t>&lt;mat1:A70*1&gt;
@@ -1449,7 +1449,7 @@
   </si>
   <si>
     <t>A dildo that imitates the tail of an incubus
-Sex toys automatic recovery of energy +1 automatic recovery of physical strength +1</t>
+Sex toys automatic recovery of energy +1 automatic recovery of HP +1</t>
   </si>
   <si>
     <t>&lt;mat1:A4*1&gt;
@@ -1728,7 +1728,7 @@
   </si>
   <si>
     <t>It's also a problem to be too late
-Rubber physical strength consumption -10%</t>
+Rubber HP consumption -10%</t>
   </si>
   <si>
     <t>無色透明な膜</t>
@@ -1770,7 +1770,7 @@
   </si>
   <si>
     <t>Medicinal rubber that relieves tiredness and stiffness
-Rubber automatic recovery of physical strength +2</t>
+Rubber automatic recovery of HP +2</t>
   </si>
   <si>
     <t>アロマゴム</t>
@@ -1784,7 +1784,7 @@
   </si>
   <si>
     <t>Rubber that refreshes the mind and body with a nice scent
-Rubber automatic recovery +2 Physical strength automatic recovery +2</t>
+Rubber automatic recovery +2 HP automatic recovery +2</t>
   </si>
   <si>
     <t>マグネティックゴム</t>
@@ -1798,7 +1798,7 @@
   </si>
   <si>
     <t>Rubber that seems to improve blood flow
-Rubber automatic recovery +2 Physical strength automatic recovery +2</t>
+Rubber automatic recovery +2 HP automatic recovery +2</t>
   </si>
   <si>
     <t>ヘルスケアゴム</t>
@@ -1812,7 +1812,7 @@
   </si>
   <si>
     <t>Rubber that is good for your body and keeps you healthy every day
-Rubber automatic recovery of physical strength +4</t>
+Rubber automatic recovery of HP +4</t>
   </si>
   <si>
     <t>再生のゴム</t>
@@ -2743,7 +2743,7 @@
   </si>
   <si>
     <t>Fairy bracelet, a ring for humans
-Ring fascination invalid, aphrodisiac poison invalid, physical strength consumption -20%</t>
+Ring fascination invalid, aphrodisiac poison invalid, HP consumption -20%</t>
   </si>
   <si>
     <t>&lt;mat1:I78*1&gt;
@@ -2800,7 +2800,7 @@
   </si>
   <si>
     <t>A ring that expresses calmness
-Ring Excitement disabled Automatic recovery of physical strength +3</t>
+Ring Excitement disabled Automatic recovery of HP +3</t>
   </si>
   <si>
     <t>&lt;mat1:I79*1&gt;
@@ -2882,7 +2882,7 @@
   </si>
   <si>
     <t>A ring that gives you strength
-Ring, weakness invalid, restraint invalid, physical strength automatic recovery +1</t>
+Ring, weakness invalid, restraint invalid, HP automatic recovery +1</t>
   </si>
   <si>
     <t>涙の指輪</t>
@@ -2938,7 +2938,7 @@
   </si>
   <si>
     <t>Black cat shop special ring limited to customers
-Ring action additional 5% maximum energy +200 maximum physical strength +20</t>
+Ring action additional 5% maximum energy +200 maximum HP +20</t>
   </si>
   <si>
     <t>成金の指輪</t>
@@ -3036,7 +3036,7 @@
   </si>
   <si>
     <t>A ring with the magical power of a famous magician
-Ring: Automatic recovery of physical strength +5</t>
+Ring: Automatic recovery of HP +5</t>
   </si>
   <si>
     <t>&lt;mat1:I793*1&gt;
@@ -3766,7 +3766,7 @@
   </si>
   <si>
     <t>Earrings that shine on the night of the crescent moon
-Accessory Automatic recovery of physical strength +1</t>
+Accessory Automatic recovery of HP +1</t>
   </si>
   <si>
     <t>半月のイヤリング</t>
@@ -3780,7 +3780,7 @@
   </si>
   <si>
     <t>Earrings that shine on a half-moon night
-Accessory Automatic recovery of physical strength +2</t>
+Accessory Automatic recovery of HP +2</t>
   </si>
   <si>
     <t>&lt;mat1:A336*1&gt;
@@ -3799,7 +3799,7 @@
   </si>
   <si>
     <t>Earrings that shine on a full moon night
-Accessory Automatic recovery of physical strength +3</t>
+Accessory Automatic recovery of HP +3</t>
   </si>
   <si>
     <t>&lt;mat1:A337*2&gt;
@@ -4204,7 +4204,7 @@
     <t>シィナのパンツ</t>
   </si>
   <si>
-    <t>Sina's pants</t>
+    <t>Shina's pants</t>
   </si>
   <si>
     <t>嗅ぐとIQが下がる

</xml_diff>

<commit_message>
Translation of Map102 (Mostly finished, moving to new maps)
</commit_message>
<xml_diff>
--- a/data/Armors.xlsx
+++ b/data/Armors.xlsx
@@ -1265,7 +1265,7 @@
 性具　悪属性特効</t>
   </si>
   <si>
-    <t>Holy vibe that seals the devil
+    <t>Holy vibe that seAlsto the devil
 Sex toys bad attributes special effects</t>
   </si>
   <si>
@@ -1306,7 +1306,7 @@
 性具　悪属性特効　毎ターン精力-1%</t>
   </si>
   <si>
-    <t>Holy vibe that seals the devil
+    <t>Holy vibe that seAlsto the devil
 Sex toys Evil attribute special effects -1% energy every turn</t>
   </si>
   <si>
@@ -1727,7 +1727,7 @@
 ゴム　体力消費-10%</t>
   </si>
   <si>
-    <t>It's also a problem to be too late
+    <t>It's Alstoo a problem to be too late
 Rubber HP consumption -10%</t>
   </si>
   <si>
@@ -1825,7 +1825,7 @@
 ゴム　精力自動回復+4</t>
   </si>
   <si>
-    <t>Rubber made from recycled materials
+    <t>Rubber made from recycled materiAlsto
 Rubber automatic recovery +4</t>
   </si>
   <si>
@@ -2112,7 +2112,7 @@
 ゴム　怯み無効</t>
   </si>
   <si>
-    <t>It is also written in the Kojiki that Shinobi used it.
+    <t>It is Alstoo written in the Kojiki that Shinobi used it.
 Rubber frightening invalid</t>
   </si>
   <si>
@@ -2357,7 +2357,7 @@
 ゴム　精力自動回復-1　催淫毒付与</t>
   </si>
   <si>
-    <t>Rubber that is charged with dangerous poison I am also dangerous
+    <t>Rubber that is charged with dangerous poison I am Alstoo dangerous
 Rubber automatic recovery-1 aphrodisiac poisoning</t>
   </si>
   <si>
@@ -3268,7 +3268,7 @@
 装飾品　防御効果+20%</t>
   </si>
   <si>
-    <t>Adventurer's essentials to protect the key points
+    <t>Adventurer's essentiAlsto to protect the key points
 Accessory defense effect + 20%</t>
   </si>
   <si>

</xml_diff>

<commit_message>
3 Scenes translated - Lime's fj, Lily's temptation, and liliy's thiighjob
</commit_message>
<xml_diff>
--- a/data/Armors.xlsx
+++ b/data/Armors.xlsx
@@ -1727,7 +1727,7 @@
 ゴム　体力消費-10%</t>
   </si>
   <si>
-    <t>It's Alstoo a problem to be too late
+    <t>It's also a problem to be too late
 Rubber HP consumption -10%</t>
   </si>
   <si>
@@ -2112,7 +2112,7 @@
 ゴム　怯み無効</t>
   </si>
   <si>
-    <t>It is Alstoo written in the Kojiki that Shinobi used it.
+    <t>It is also written in the Kojiki that Shinobi used it.
 Rubber frightening invalid</t>
   </si>
   <si>
@@ -2357,7 +2357,7 @@
 ゴム　精力自動回復-1　催淫毒付与</t>
   </si>
   <si>
-    <t>Rubber that is charged with dangerous poison I am Alstoo dangerous
+    <t>Rubber that is charged with dangerous poison I am also dangerous
 Rubber automatic recovery-1 aphrodisiac poisoning</t>
   </si>
   <si>
@@ -4358,7 +4358,7 @@
     <t>ロメリアの髪飾り</t>
   </si>
   <si>
-    <t>Romeria hair ornament</t>
+    <t>Meria hair ornament</t>
   </si>
   <si>
     <t>大事な妹の髪飾り

</xml_diff>